<commit_message>
Added CaseDefendantParty and MessageOperationCode to CourtEvent
</commit_message>
<xml_diff>
--- a/schemas/CourtEvent_iepd/artifacts/CourtEvent_MappingSpreadsheet.xlsx
+++ b/schemas/CourtEvent_iepd/artifacts/CourtEvent_MappingSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcp911gov-my.sharepoint.com/personal/aidandelgado_missioncriticalpartners_com/Documents/ONE.WORKSPACE/21. NOLA/EXCHANGES/COURT EVENT/Mapping Spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\CourtEvent_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{577A8D05-6F3C-460B-8427-0A518FE8834F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C68386-71A0-4D95-BB4B-6E8C81E921EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="0" windowWidth="23490" windowHeight="15600" xr2:uid="{6CF1A792-55F6-4EFF-A83A-261B71252191}"/>
+    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{6CF1A792-55F6-4EFF-A83A-261B71252191}"/>
   </bookViews>
   <sheets>
     <sheet name="Court Event" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="486">
   <si>
     <t>Property Type</t>
   </si>
@@ -1426,12 +1426,380 @@
   <si>
     <t>/Person/PersonName/PersonNamePrefixText</t>
   </si>
+  <si>
+    <t>MessageOperationCode</t>
+  </si>
+  <si>
+    <t>A type of message operation.</t>
+  </si>
+  <si>
+    <t>nola-ext:MessageOperationCode</t>
+  </si>
+  <si>
+    <t>nc:MetadaType</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>Defendant</t>
+  </si>
+  <si>
+    <t>A person who is the subject of an investigation or alleged offense. An entity being charged or sued in a court of law.</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>CaseDefendantNumber</t>
+  </si>
+  <si>
+    <t>A defandant number associated with a specific criminal court case number.</t>
+  </si>
+  <si>
+    <t>[{"db": "AS400_CDC_CMS",	"table": "CASEVT",	"fieldDesc": "CourtCaseDefendantNumber",	"field": "CVCDEF"},
+{"db": "AS400_CDC_CMS",	"table": "CASEVT_CASEVD_UNION",	"fieldDesc": "CourtCaseDefendantNumber",	"field": "CVCDEF"},
+{"db": "AS400_CDC_CMS",	"table": "CHRGLOG",	"fieldDesc": "CourtCaseDefendantNumber",	"field": "CXDEF#"},
+{"db": "AS400_CDC_CMS",	"table": "DEFCHG",	"fieldDesc": "CourtCaseDefendantNumber",	"field": "DCCDEF"},
+{"db": "AS400_CDC_CMS",	"table": "SENTLOG",	"fieldDesc": "CourtCaseDefendantNumber",	"field": "SXDEF#"},
+{"db": "AS400_CDC_CMS",	"table": "CASEVD",	"fieldDesc": "CourtDefendantNumber",	"field": "CXCDEF"},
+{"db": "EPR",		"table": "Gists",	"fieldDesc": "OffenderID",			"field": "OffenderID"},
+{"db": "EPR",		"table": "OffenderCharges",	"fieldDesc": "OffenderID",		"field": "OffenderID"},
+{"db": "EPR",		"table": "Offenders",	"fieldDesc": "OffenderID",		"field": "OffenderID"},
+{"db": "EPR",		"table": "Offenders",	"fieldDesc": "OffenderNumber",	"field":OffenderNumber"},
+{"db": "AS400_CDC_CMS",	"table": "PARTIES",	"fieldDesc": "DefendantNumber",	"field": "PCDEF"},
+{"db": "MC",		"table": "Digicourt_Orleans.dbview.vw_ArrestDetail",	"fieldDesc": "DefendantID",	"field": "DEF_ID"},
+{"db": "MC",		"table": "Digicourt_Orleans.dbview.vw_CriminalCaseFileDetail",	"fieldDesc": "DefendantID",	"field": "DEF_ID"},
+{"db": "MC",		"table": "DigiCourt_Orleans.dbview.vw_AllWarrants",	"fieldDesc": "DefendantID",	"field": "DEF_ID"}]</t>
+  </si>
+  <si>
+    <t>nola-ext:CaseDefendantNumber</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>OffenderDescription</t>
+  </si>
+  <si>
+    <t>A description of a person.</t>
+  </si>
+  <si>
+    <t>[{"db": "EPR",	"table": "Offenders",	"fieldDesc": "AdditionalDescription",	"field": "AdditionalDescription"}]</t>
+  </si>
+  <si>
+    <t>nc:PersonDescriptionText</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/j:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/j:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nola-ext:PersonAugmentation/nola-ext:CaseDefendantNumber</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/j:CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonDescriptionText</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>PersonIdentifiers</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>A date a person was born.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "DateofBirth",	"field": "IDDOBD"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "Witness1DateofBirth",	"field": "IDDOBDW1"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "Witness2DateofBirth",	"field": "IDDOBDW2"},
+{"db": "AS400_JMS",	"table": "IMARRD_ChargesAll_w_Keys",	"fieldDesc": "DateofBirth",	"field": "Date_of_Birth"},
+{"db": "AS400_JMS",	"table": "IMMSTR",	"fieldDesc": "DateofBirth",	"field": "IMDOBD"},
+{"db": "AS400_JMS",	"table": "IMFLDR",	"fieldDesc": "DateofBirth",	"field": "IFDOBD"},
+{"db": "AS400_CDC_CMS",	"table": "DEFEND",	"fieldDesc": "DateofBirth",	"field": "DEDOB"},
+{"db": "EPR",	"table": "Offenders",	"fieldDesc": "DateOfBirth",	"field": "DateOfBirth"},
+{"db": "EPR",	"table": "VictimPersons",	"fieldDesc": "DateOfBirth",	"field": "DateOfBirth"},
+{"db": "MC",	"table": "Digicourt_Orleans.dbview.vw_ArrestDetail",	"fieldDesc": "DateofBirth",	"field": "   DOB"},
+{"db": "MC",	"table": "[DigiCourt_Orleans].[dbview].vw_AllWarrants",	"fieldDesc": "DateofBirth",	"field": "      DOB"},
+{"db": "MC",	"table": "Digicourt_Orleans.dbview.vw_CriminalCaseFileDetail",	"fieldDesc": "Race",	"field": "DOB"}]
+</t>
+  </si>
+  <si>
+    <t>nc:Date</t>
+  </si>
+  <si>
+    <t>niem-xs:date</t>
+  </si>
+  <si>
+    <t>/nc:CourtCase/nc:CaseAugmentationPoint/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonBirthDate/nc:DateRepresentation/nc:Date</t>
+  </si>
+  <si>
+    <t>/nola:EntityUpdateExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/EntityPerson/PersonBirthDate</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>InmateNumber</t>
+  </si>
+  <si>
+    <t>An identifier assigned to the detainee by the detention facility.</t>
+  </si>
+  <si>
+    <t>scr:InmateNumberID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nola-ext:DefendantAugmentationType/nola-ext:InmateDefendant
+</t>
+  </si>
+  <si>
+    <t>/nola:EntityUpdateExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/EntityPerson/nola-ext:PersonAugmentation/scr:InmateNumberID</t>
+  </si>
+  <si>
+    <t>249</t>
+  </si>
+  <si>
+    <t>SIDNumber</t>
+  </si>
+  <si>
+    <t>A person, organization, or locale which issues an identification. For example Sheriff's ID number</t>
+  </si>
+  <si>
+    <t>[{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "SIDNumber",	"field": "IDSIDN"},
+{"db": "AS400_JMS",	"table": "IMMSTR",	"fieldDesc": "SIDNumber",	"field": "IMSIDN"},
+{"db": "AS400_JMS",	"table": "IMFLDR",	"fieldDesc": "SIDNumber",	"field": "IFSIDN"},
+{"db": "AS400_CDC_CMS",	"table": "DEFEND",	"fieldDesc": "SIDNumber",	"field": "DESIDN"},
+{"db": "CASTNetDB",	"table": "PersonSid",	"fieldDesc": "Sid",	"field": "Sid"}]</t>
+  </si>
+  <si>
+    <t>/j:BookingSubject/RoleOfPerson/PersonStateIdentification/IdentificationID
+/EntityPerson/PersonStateIdentification/IdentificationID</t>
+  </si>
+  <si>
+    <t>/nola:EntityUpdateExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/EntityPerson/PersonStateIdentification/IdentificationID</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>SocialSecurityNumber</t>
+  </si>
+  <si>
+    <t>A unique identification reference to a living person; assigned by the United States Social Security Administration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "SocialSecurityNumber",	"field": "IDSSNO"},
+{"db": "AS400_JMS",	"table": "IMMSTR",	"fieldDesc": "SocialSecurityNumber",	"field": "IMSSNO"},
+{"db": "AS400_JMS",	"table": "IMFLDR",	"fieldDesc": "SocialSecurityNumber",	"field": "IFSSNO"},
+{"db": "EPR",	"table": 	"Offenders",		"fieldDesc": "SocialSecurityNumber",	"field": "SocialSecurityNumber"},
+{"db": "EPR",	"table": 	"VictimPersons",	"fieldDesc": "SocialSecurityNumber",	"field": "SocialSecurityNumber"},
+{"db": "CASTNetDB",	"table": "PersonSsn",	"fieldDesc": "Ssn",		"field": "Ssn"},
+{"db": "CASTNetDB",	"table": "vw_Person",	"fieldDesc": "Ssn",		"field": "Ssn"},
+{"db": "MC",	"table": "Digicourt_Orleans.dbview.vw_ArrestDetail",	"fieldDesc": "SocialSecurityNumber",	"field": "SSN"},
+{"db": "MC",	"table": "Digicourt_Orleans.dbview.vw_CriminalCaseFileDetail",	"fieldDesc": "SocialSecurityNumber",	"field": "SSN"},
+{"db": "MC",	"table": "DigiCourt_Orleans.dbview.vw_AllWarrants",	"fieldDesc": "SocialSecurityNumber",	"field": "SSN"}]
+</t>
+  </si>
+  <si>
+    <t>/Person/PersonSSNIdentification/IdentificationID
+/j:CaseDefendantParty/EntityPerson/PersonSSNIdentification/IdentificationID</t>
+  </si>
+  <si>
+    <t>/nola:EntityUpdateExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/EntityPerson/PersonSSNIdentification</t>
+  </si>
+  <si>
+    <t>Employer</t>
+  </si>
+  <si>
+    <t>EmployerName</t>
+  </si>
+  <si>
+    <t>A name of an employer.</t>
+  </si>
+  <si>
+    <t>[{"db": "AS400_JMS",	"table": "IMMSTR",	"fieldDesc": "Employer",	"field": "IMEMPR"},
+{"db": "AS400_JMS",	"table": "IMFLDR",	"fieldDesc": "Employer",	"field": "IFEMPR"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "Employer",	"field": "IDEMPR"}]</t>
+  </si>
+  <si>
+    <t>hs:EmployerName</t>
+  </si>
+  <si>
+    <t>/RoleOfPerson/nola-ext:PersonAugmentation/PersonEmploymentAssociation/Employer/hs:EmployerAugmentation/hs:EmployerName</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/EntityPerson/nola-ext:PersonAugmentation/PersonEmploymentAssociation/Employer/hs:EmployerAugmentation/hs:EmployerName</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>EmploymentStatusText</t>
+  </si>
+  <si>
+    <t>A description of a status or condition of employment.</t>
+  </si>
+  <si>
+    <t>[{"db": "AS400_JMS",	"table": "IMMISC",	"fieldDesc": "EmploymentStatusText",	"field": "MSEMPT"}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nc:StatusDescriptionText </t>
+  </si>
+  <si>
+    <t>/RoleOfPerson/nola-ext:PersonAugmentation/PersonEmploymentAssociation/Employer/nola-ext:EmployerAugmentation/EmploymentStatus/StatusDescriptionText
+/EntityPerson/nola-ext:PersonAugmentation/PersonEmploymentAssociation/EmploymentStatus/StatusDescriptionText</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/EntityPerson/nola-ext:PersonAugmentation/PersonEmploymentAssociation/EmploymentStatus/StatusDescriptionText</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>PersonDemographics</t>
+  </si>
+  <si>
+    <t>Features describing a person.</t>
+  </si>
+  <si>
+    <t>211</t>
+  </si>
+  <si>
+    <t>GenderText</t>
+  </si>
+  <si>
+    <t>A gender or sex of a person.</t>
+  </si>
+  <si>
+    <t>[{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "GenderCode",	"field": "IDSEXC"},
+{"db": "AS400_JMS",	"table": "IMMSTR",	"fieldDesc": "GenderCode",	"field": "IMSEXC"},
+{"db": "AS400_CDC_CMS",	"table": "DEFEND",	"fieldDesc": "GenderCode",	"field": "DESEX"},
+{"db": "CASTNetDB",		"table": "vw_Person",	"fieldDesc": "GenderCode",	"field": "GenderCode"},
+{"db": "EPR",	"table": "Offenders",	"fieldDesc": "GenderTypeID",	"field": "GenderTypeID"},
+{"db": "EPR",	"table": "VictimPersons",	"fieldDesc": "GenderTypeID",	"field": "GenderTypeID"},
+{"db": "EPR",	"table": "GenderTypes",	"fieldDesc": "MainframeCode",	"field": "MainframeCode"},
+{"db": "CASTNetDB",	"table": "Person",	"fieldDesc": "GenderId",	"field": "GenderId"}]</t>
+  </si>
+  <si>
+    <t>nc:PersonSexText</t>
+  </si>
+  <si>
+    <t>/RoleOfPerson/hs:PersonAugmentation/hs:PersonGenderIdentityText
+/EntityPerson/PersonSexText</t>
+  </si>
+  <si>
+    <t>/nola:EntityUpdateExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/EntityPerson/PersonSexText</t>
+  </si>
+  <si>
+    <t>209</t>
+  </si>
+  <si>
+    <t>RaceText</t>
+  </si>
+  <si>
+    <t>A classification of a person based on factors such as geographical locations and genetics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "RaceCode",	"field": "IDRACE"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "Witness1RaceCode",	"field": "IDRACEW1"},
+{"db": "AS400_JMS",	"table": "IMARRD",	"fieldDesc": "Witness2RaceCode",	"field": "IDRACEW2"},
+{"db": "AS400_JMS",	"table": "IMARRD_ChargesAll_w_Keys",	"fieldDesc": "Race",	"field": "Race"},
+{"db": "AS400_JMS",	"table": "IMFLDR",	"fieldDesc": "Race",	"field": "IFRACE"},
+{"db": "AS400_JMS",	"table": "IMMSTR",	"fieldDesc": "RaceCode",	"field": "IMRACE"},
+{"db": "AS400_CDC_CMS","table": "DEFEND",	"fieldDesc": "RaceCode",	"field": "DERACE"},
+{"db": "EPR",	"table": "Offenders",	"fieldDesc": "RaceTypeID",	"field": "RaceTypeID"},
+{"db": "EPR",	"table": "VictimPersons",	"fieldDesc": "RaceTypeID",	"field": "RaceTypeID"},
+{"db": "EPR",	"table": "RaceTypes",		"fieldDesc": "Description",	"field": "Description"},
+{"db": "CASTNetDB",	"table": "vw_Person",	"fieldDesc": "RaceCode",	"field": "RaceCode"},
+{"db": "CASTNetDB",	"table": "PersonAlias",		"fieldDesc": "Race",	"field": "Race"},
+{"db": "CASTNetDB",	"table": "PersonNickName",	"fieldDesc": "Race",	"field": "Race"},
+{"db": "CASTNetDB",	"table": "vw_Person",		"fieldDesc": "Race",	"field": "Race"},
+{"db": "MC",	"table": "Digicourt_Orleans.dbview.vw_CriminalCaseFileDetail",	"fieldDesc": "Gender",	"field": "      RACE"},
+{"db": "MC",	"table": "Digicourt_Orleans.dbview.vw_ArrestDetail",	"fieldDesc": "Race",	"field": "RACE"},
+{"db": "MC",	"table": "DigiCourt_Orleans.dbview.vw_AllWarrants",	"fieldDesc": "Race",	"field": "RACE"},
+{"db": "EPR",	"table": "RaceTypes",	"fieldDesc": "Description",	"field": "Description"}]
+</t>
+  </si>
+  <si>
+    <t>nc:PersonRaceText</t>
+  </si>
+  <si>
+    <t>/Person/PersonRaceText
+/EntityPerson/PersonRaceText</t>
+  </si>
+  <si>
+    <t>/nola:EntityUpdateExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/EntityPerson/PersonRaceText</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>USCitizenship</t>
+  </si>
+  <si>
+    <t>True if a person is a citizen of the United States; false otherwise.</t>
+  </si>
+  <si>
+    <t>[{"db": "AS400_JMS",	"table": "IMMSTR",	"fieldDesc": "USCitizenship",	"field": "IMUSAC"},
+{"db": "AS400_JMS",	"table": "IMFLDR",	"fieldDesc": "USCitizenship",	"field": "IFUSAC"}]</t>
+  </si>
+  <si>
+    <t>nc:PersonUSCitizenIndicator</t>
+  </si>
+  <si>
+    <t>niem-xs:boolean</t>
+  </si>
+  <si>
+    <t>/Person/PersonUSCitizenIndicator
+/EntityPerson/PersonUSCitizenIndicator</t>
+  </si>
+  <si>
+    <t>/nola:EntityUpdateExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/EntityPerson/PersonUSCitizenIndicator</t>
+  </si>
+  <si>
+    <t>236</t>
+  </si>
+  <si>
+    <t>A collection of identifiers related to a defendant in a criminal court proceeding.</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonUSCitizenIndicator</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonRaceText</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonSexText</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonBirthDate</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/EntityPerson/nola-ext:PersonAugmentation/scr:InmateNumberID</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonSSNIdentification</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/nola-ext:MessageOperationCode</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/nc:PersonStateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/EntityPerson/nola-ext:PersonAugmentation/nc:PersonEmploymentAssociation/nc:Employer/hs:EmployerAugmentation/hs:EmployerName</t>
+  </si>
+  <si>
+    <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/EntityPerson/nola-ext:PersonAugmentation/nc:PersonEmploymentAssociation/nc:EmploymentStatus/nc:StatusDescriptionText</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1450,8 +1818,21 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1472,6 +1853,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79995117038483843"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1564,7 +1951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1606,6 +1993,22 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2066,13 +2469,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2105,6 +2501,13 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2148,7 +2551,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D1C00DE-EF4F-483A-9AEE-9A164B2AF960}" name="MappingSpreadsheet" displayName="MappingSpreadsheet" ref="A1:O78" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D1C00DE-EF4F-483A-9AEE-9A164B2AF960}" name="MappingSpreadsheet" displayName="MappingSpreadsheet" ref="A1:O78" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A1:O78" xr:uid="{B09137D3-E1F4-4790-A6C1-6986B28644D7}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{DDD07387-8786-4201-81D4-D049D1BB39CD}" name="Property Type" dataDxfId="14"/>
@@ -2469,29 +2872,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18CFC728-CFAD-4708-B4DA-65E1AE154AFA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O78"/>
+  <dimension ref="A1:O93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="I59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q10" sqref="Q10"/>
+      <selection pane="bottomRight" activeCell="L93" sqref="L93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.86328125" customWidth="1"/>
+    <col min="2" max="2" width="5.1328125" customWidth="1"/>
+    <col min="3" max="3" width="12.86328125" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.86328125" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="100.85546875" customWidth="1"/>
-    <col min="10" max="15" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.59765625" customWidth="1"/>
+    <col min="9" max="9" width="100.86328125" customWidth="1"/>
+    <col min="10" max="15" width="11.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2538,7 +2941,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2573,7 +2976,7 @@
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -2606,7 +3009,7 @@
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
     </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2647,7 +3050,7 @@
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="10" t="s">
         <v>35</v>
       </c>
@@ -2684,7 +3087,7 @@
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -2721,7 +3124,7 @@
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -2758,7 +3161,7 @@
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
@@ -2795,7 +3198,7 @@
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
     </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
@@ -2832,7 +3235,7 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
@@ -2865,7 +3268,7 @@
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
     </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
@@ -2900,7 +3303,7 @@
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
         <v>3</v>
       </c>
@@ -2937,7 +3340,7 @@
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
         <v>3</v>
       </c>
@@ -2978,7 +3381,7 @@
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
         <v>3</v>
       </c>
@@ -3019,7 +3422,7 @@
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>3</v>
       </c>
@@ -3060,7 +3463,7 @@
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>3</v>
       </c>
@@ -3101,7 +3504,7 @@
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
     </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>3</v>
       </c>
@@ -3142,7 +3545,7 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>3</v>
       </c>
@@ -3177,7 +3580,7 @@
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
     </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
         <v>3</v>
       </c>
@@ -3214,7 +3617,7 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
     </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
         <v>3</v>
       </c>
@@ -3251,7 +3654,7 @@
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
     </row>
-    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
@@ -3286,7 +3689,7 @@
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
         <v>3</v>
       </c>
@@ -3319,7 +3722,7 @@
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
         <v>3</v>
       </c>
@@ -3360,7 +3763,7 @@
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
     </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
         <v>3</v>
       </c>
@@ -3395,7 +3798,7 @@
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
     </row>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="7" t="s">
         <v>3</v>
       </c>
@@ -3428,7 +3831,7 @@
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
     </row>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="7" t="s">
         <v>3</v>
       </c>
@@ -3469,7 +3872,7 @@
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
     </row>
-    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="7" t="s">
         <v>3</v>
       </c>
@@ -3510,7 +3913,7 @@
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
     </row>
-    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="7" t="s">
         <v>3</v>
       </c>
@@ -3545,7 +3948,7 @@
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
     </row>
-    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="7" t="s">
         <v>3</v>
       </c>
@@ -3578,7 +3981,7 @@
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
     </row>
-    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="7" t="s">
         <v>3</v>
       </c>
@@ -3621,7 +4024,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="10" t="s">
         <v>35</v>
       </c>
@@ -3652,7 +4055,7 @@
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
     </row>
-    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="7" t="s">
         <v>3</v>
       </c>
@@ -3687,7 +4090,7 @@
       <c r="N32" s="9"/>
       <c r="O32" s="9"/>
     </row>
-    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="7" t="s">
         <v>3</v>
       </c>
@@ -3722,7 +4125,7 @@
       <c r="N33" s="9"/>
       <c r="O33" s="9"/>
     </row>
-    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="7" t="s">
         <v>3</v>
       </c>
@@ -3757,7 +4160,7 @@
       <c r="N34" s="9"/>
       <c r="O34" s="9"/>
     </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="7" t="s">
         <v>3</v>
       </c>
@@ -3798,7 +4201,7 @@
       <c r="N35" s="9"/>
       <c r="O35" s="9"/>
     </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="7" t="s">
         <v>3</v>
       </c>
@@ -3831,7 +4234,7 @@
       <c r="N36" s="9"/>
       <c r="O36" s="9"/>
     </row>
-    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="7" t="s">
         <v>3</v>
       </c>
@@ -3874,7 +4277,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="7" t="s">
         <v>3</v>
       </c>
@@ -3913,7 +4316,7 @@
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
     </row>
-    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="7" t="s">
         <v>3</v>
       </c>
@@ -3956,7 +4359,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="7" t="s">
         <v>3</v>
       </c>
@@ -3989,7 +4392,7 @@
       <c r="N40" s="9"/>
       <c r="O40" s="9"/>
     </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
@@ -4024,7 +4427,7 @@
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
     </row>
-    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="7" t="s">
         <v>3</v>
       </c>
@@ -4065,7 +4468,7 @@
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
     </row>
-    <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="7" t="s">
         <v>3</v>
       </c>
@@ -4098,7 +4501,7 @@
       <c r="N43" s="9"/>
       <c r="O43" s="9"/>
     </row>
-    <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="7" t="s">
         <v>3</v>
       </c>
@@ -4133,7 +4536,7 @@
       <c r="N44" s="9"/>
       <c r="O44" s="9"/>
     </row>
-    <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
         <v>3</v>
       </c>
@@ -4166,7 +4569,7 @@
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
     </row>
-    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="7" t="s">
         <v>3</v>
       </c>
@@ -4199,7 +4602,7 @@
       <c r="N46" s="9"/>
       <c r="O46" s="9"/>
     </row>
-    <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="7" t="s">
         <v>3</v>
       </c>
@@ -4232,7 +4635,7 @@
       <c r="N47" s="9"/>
       <c r="O47" s="9"/>
     </row>
-    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="7" t="s">
         <v>3</v>
       </c>
@@ -4265,7 +4668,7 @@
       <c r="N48" s="9"/>
       <c r="O48" s="9"/>
     </row>
-    <row r="49" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="7" t="s">
         <v>3</v>
       </c>
@@ -4298,7 +4701,7 @@
       <c r="N49" s="9"/>
       <c r="O49" s="9"/>
     </row>
-    <row r="50" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="7" t="s">
         <v>3</v>
       </c>
@@ -4331,7 +4734,7 @@
       <c r="N50" s="9"/>
       <c r="O50" s="9"/>
     </row>
-    <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="7" t="s">
         <v>3</v>
       </c>
@@ -4364,7 +4767,7 @@
       <c r="N51" s="9"/>
       <c r="O51" s="9"/>
     </row>
-    <row r="52" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="7" t="s">
         <v>3</v>
       </c>
@@ -4397,7 +4800,7 @@
       <c r="N52" s="9"/>
       <c r="O52" s="9"/>
     </row>
-    <row r="53" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
@@ -4432,7 +4835,7 @@
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
     </row>
-    <row r="54" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="7" t="s">
         <v>3</v>
       </c>
@@ -4473,7 +4876,7 @@
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
     </row>
-    <row r="55" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="10" t="s">
         <v>35</v>
       </c>
@@ -4510,7 +4913,7 @@
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
     </row>
-    <row r="56" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="7" t="s">
         <v>3</v>
       </c>
@@ -4551,7 +4954,7 @@
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
     </row>
-    <row r="57" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
         <v>2</v>
       </c>
@@ -4580,7 +4983,7 @@
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
     </row>
-    <row r="58" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="10" t="s">
         <v>35</v>
       </c>
@@ -4617,7 +5020,7 @@
       <c r="N58" s="9"/>
       <c r="O58" s="9"/>
     </row>
-    <row r="59" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="10" t="s">
         <v>35</v>
       </c>
@@ -4648,7 +5051,7 @@
       <c r="N59" s="9"/>
       <c r="O59" s="9"/>
     </row>
-    <row r="60" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
         <v>2</v>
       </c>
@@ -4679,7 +5082,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="7" t="s">
         <v>3</v>
       </c>
@@ -4720,7 +5123,7 @@
       <c r="N61" s="9"/>
       <c r="O61" s="9"/>
     </row>
-    <row r="62" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="7" t="s">
         <v>3</v>
       </c>
@@ -4761,7 +5164,7 @@
       <c r="N62" s="9"/>
       <c r="O62" s="9"/>
     </row>
-    <row r="63" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
         <v>2</v>
       </c>
@@ -4796,7 +5199,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="10" t="s">
         <v>35</v>
       </c>
@@ -4833,7 +5236,7 @@
       <c r="N64" s="9"/>
       <c r="O64" s="9"/>
     </row>
-    <row r="65" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>2</v>
       </c>
@@ -4862,7 +5265,7 @@
       <c r="N65" s="4"/>
       <c r="O65" s="4"/>
     </row>
-    <row r="66" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
         <v>2</v>
       </c>
@@ -4891,7 +5294,7 @@
       <c r="N66" s="4"/>
       <c r="O66" s="4"/>
     </row>
-    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="7" t="s">
         <v>3</v>
       </c>
@@ -4932,7 +5335,7 @@
       <c r="N67" s="9"/>
       <c r="O67" s="9"/>
     </row>
-    <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="10" t="s">
         <v>35</v>
       </c>
@@ -4971,7 +5374,7 @@
       <c r="N68" s="9"/>
       <c r="O68" s="9"/>
     </row>
-    <row r="69" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
         <v>2</v>
       </c>
@@ -5006,7 +5409,7 @@
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
     </row>
-    <row r="70" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="7" t="s">
         <v>3</v>
       </c>
@@ -5049,7 +5452,7 @@
       <c r="N70" s="9"/>
       <c r="O70" s="9"/>
     </row>
-    <row r="71" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="7" t="s">
         <v>3</v>
       </c>
@@ -5092,7 +5495,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="7" t="s">
         <v>3</v>
       </c>
@@ -5133,7 +5536,7 @@
       <c r="N72" s="9"/>
       <c r="O72" s="9"/>
     </row>
-    <row r="73" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="7" t="s">
         <v>3</v>
       </c>
@@ -5176,7 +5579,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="7" t="s">
         <v>3</v>
       </c>
@@ -5219,7 +5622,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="7" t="s">
         <v>3</v>
       </c>
@@ -5262,7 +5665,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="7" t="s">
         <v>3</v>
       </c>
@@ -5303,7 +5706,7 @@
       <c r="N76" s="9"/>
       <c r="O76" s="9"/>
     </row>
-    <row r="77" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="7" t="s">
         <v>3</v>
       </c>
@@ -5340,7 +5743,7 @@
       <c r="N77" s="9"/>
       <c r="O77" s="9"/>
     </row>
-    <row r="78" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="12" t="s">
         <v>3</v>
       </c>
@@ -5380,6 +5783,604 @@
       <c r="M78" s="14"/>
       <c r="N78" s="14"/>
       <c r="O78" s="14"/>
+    </row>
+    <row r="79" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A79" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="E79" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F79" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="G79" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="H79" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="I79" s="16"/>
+      <c r="J79" s="16" t="s">
+        <v>390</v>
+      </c>
+      <c r="K79" s="16" t="s">
+        <v>391</v>
+      </c>
+      <c r="L79" s="16" t="s">
+        <v>482</v>
+      </c>
+      <c r="M79" s="16"/>
+      <c r="N79" s="16"/>
+      <c r="O79" s="18"/>
+    </row>
+    <row r="80" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A80" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="19" t="s">
+        <v>392</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="D80" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E80" s="20"/>
+      <c r="F80" s="19" t="s">
+        <v>394</v>
+      </c>
+      <c r="G80" s="20"/>
+      <c r="H80" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="I80" s="19"/>
+      <c r="J80" s="19"/>
+      <c r="K80" s="19"/>
+      <c r="L80" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="M80" s="19"/>
+      <c r="N80" s="19"/>
+      <c r="O80" s="18"/>
+    </row>
+    <row r="81" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A81" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" s="19" t="s">
+        <v>395</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="D81" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F81" s="19" t="s">
+        <v>397</v>
+      </c>
+      <c r="G81" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H81" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="I81" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="J81" s="19" t="s">
+        <v>399</v>
+      </c>
+      <c r="K81" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="L81" s="19" t="s">
+        <v>406</v>
+      </c>
+      <c r="M81" s="18"/>
+      <c r="N81" s="18"/>
+      <c r="O81" s="18"/>
+    </row>
+    <row r="82" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A82" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="C82" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="D82" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F82" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="G82" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H82" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="I82" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="J82" s="19" t="s">
+        <v>404</v>
+      </c>
+      <c r="K82" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="L82" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="M82" s="19"/>
+      <c r="N82" s="19"/>
+      <c r="O82" s="18"/>
+    </row>
+    <row r="83" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A83" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>449</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="D83" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E83" s="20"/>
+      <c r="F83" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="G83" s="20"/>
+      <c r="H83" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="I83" s="19"/>
+      <c r="J83" s="19"/>
+      <c r="K83" s="19"/>
+      <c r="L83" s="19"/>
+      <c r="M83" s="19"/>
+      <c r="N83" s="19"/>
+    </row>
+    <row r="84" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A84" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" s="19" t="s">
+        <v>452</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="D84" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E84" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F84" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="G84" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H84" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="I84" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="J84" s="19" t="s">
+        <v>456</v>
+      </c>
+      <c r="K84" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="L84" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="M84" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="N84" s="19" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A85" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" s="19" t="s">
+        <v>459</v>
+      </c>
+      <c r="C85" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="D85" s="19" t="s">
+        <v>460</v>
+      </c>
+      <c r="E85" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F85" s="19" t="s">
+        <v>461</v>
+      </c>
+      <c r="G85" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H85" s="19" t="s">
+        <v>460</v>
+      </c>
+      <c r="I85" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="J85" s="19" t="s">
+        <v>463</v>
+      </c>
+      <c r="K85" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="L85" s="19" t="s">
+        <v>477</v>
+      </c>
+      <c r="M85" s="19" t="s">
+        <v>464</v>
+      </c>
+      <c r="N85" s="19" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A86" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="C86" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="D86" s="19" t="s">
+        <v>467</v>
+      </c>
+      <c r="E86" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F86" s="19" t="s">
+        <v>468</v>
+      </c>
+      <c r="G86" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H86" s="19" t="s">
+        <v>467</v>
+      </c>
+      <c r="I86" s="19" t="s">
+        <v>469</v>
+      </c>
+      <c r="J86" s="19" t="s">
+        <v>470</v>
+      </c>
+      <c r="K86" s="19" t="s">
+        <v>471</v>
+      </c>
+      <c r="L86" s="19" t="s">
+        <v>476</v>
+      </c>
+      <c r="M86" s="19" t="s">
+        <v>472</v>
+      </c>
+      <c r="N86" s="19" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A87" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87" s="19" t="s">
+        <v>474</v>
+      </c>
+      <c r="C87" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="D87" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E87" s="20"/>
+      <c r="F87" s="19" t="s">
+        <v>475</v>
+      </c>
+      <c r="G87" s="20"/>
+      <c r="H87" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="I87" s="19"/>
+      <c r="J87" s="19"/>
+      <c r="K87" s="19"/>
+      <c r="L87" s="19"/>
+      <c r="M87" s="19"/>
+      <c r="N87" s="19"/>
+    </row>
+    <row r="88" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A88" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" s="19" t="s">
+        <v>408</v>
+      </c>
+      <c r="C88" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="D88" s="19" t="s">
+        <v>410</v>
+      </c>
+      <c r="E88" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="F88" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="G88" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H88" s="19" t="s">
+        <v>410</v>
+      </c>
+      <c r="I88" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="J88" s="19" t="s">
+        <v>413</v>
+      </c>
+      <c r="K88" s="19" t="s">
+        <v>414</v>
+      </c>
+      <c r="L88" s="19" t="s">
+        <v>479</v>
+      </c>
+      <c r="M88" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="N88" s="19" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A89" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89" s="19" t="s">
+        <v>417</v>
+      </c>
+      <c r="C89" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="D89" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="E89" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F89" s="19" t="s">
+        <v>419</v>
+      </c>
+      <c r="G89" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H89" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="I89" s="19"/>
+      <c r="J89" s="19" t="s">
+        <v>420</v>
+      </c>
+      <c r="K89" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="L89" s="19" t="s">
+        <v>480</v>
+      </c>
+      <c r="M89" s="19" t="s">
+        <v>421</v>
+      </c>
+      <c r="N89" s="19" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A90" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" s="19" t="s">
+        <v>423</v>
+      </c>
+      <c r="C90" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="D90" s="19" t="s">
+        <v>424</v>
+      </c>
+      <c r="E90" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F90" s="19" t="s">
+        <v>425</v>
+      </c>
+      <c r="G90" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H90" s="19" t="s">
+        <v>424</v>
+      </c>
+      <c r="I90" s="19" t="s">
+        <v>426</v>
+      </c>
+      <c r="J90" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K90" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="L90" s="19" t="s">
+        <v>483</v>
+      </c>
+      <c r="M90" s="19" t="s">
+        <v>427</v>
+      </c>
+      <c r="N90" s="19" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A91" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="C91" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="D91" s="19" t="s">
+        <v>430</v>
+      </c>
+      <c r="E91" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F91" s="19" t="s">
+        <v>431</v>
+      </c>
+      <c r="G91" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H91" s="19" t="s">
+        <v>430</v>
+      </c>
+      <c r="I91" s="19" t="s">
+        <v>432</v>
+      </c>
+      <c r="J91" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K91" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="L91" s="19" t="s">
+        <v>481</v>
+      </c>
+      <c r="M91" s="19" t="s">
+        <v>433</v>
+      </c>
+      <c r="N91" s="19" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A92" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C92" s="19" t="s">
+        <v>435</v>
+      </c>
+      <c r="D92" s="19" t="s">
+        <v>436</v>
+      </c>
+      <c r="E92" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F92" s="19" t="s">
+        <v>437</v>
+      </c>
+      <c r="G92" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H92" s="19" t="s">
+        <v>436</v>
+      </c>
+      <c r="I92" s="19" t="s">
+        <v>438</v>
+      </c>
+      <c r="J92" s="19" t="s">
+        <v>439</v>
+      </c>
+      <c r="K92" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="L92" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="M92" s="19" t="s">
+        <v>440</v>
+      </c>
+      <c r="N92" s="19" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A93" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93" s="19" t="s">
+        <v>442</v>
+      </c>
+      <c r="C93" s="19" t="s">
+        <v>435</v>
+      </c>
+      <c r="D93" s="19" t="s">
+        <v>443</v>
+      </c>
+      <c r="E93" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F93" s="19" t="s">
+        <v>444</v>
+      </c>
+      <c r="G93" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H93" s="19" t="s">
+        <v>443</v>
+      </c>
+      <c r="I93" s="19" t="s">
+        <v>445</v>
+      </c>
+      <c r="J93" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="K93" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="L93" s="19" t="s">
+        <v>485</v>
+      </c>
+      <c r="M93" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="N93" s="19" t="s">
+        <v>448</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added CourtEventTypeText and CourtEventSequenceID to CourtEvent
</commit_message>
<xml_diff>
--- a/schemas/CourtEvent_iepd/artifacts/CourtEvent_MappingSpreadsheet.xlsx
+++ b/schemas/CourtEvent_iepd/artifacts/CourtEvent_MappingSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\CourtEvent_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C68386-71A0-4D95-BB4B-6E8C81E921EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2336F03-3B0E-41A9-AEF0-4F2580DA72D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{6CF1A792-55F6-4EFF-A83A-261B71252191}"/>
+    <workbookView xWindow="14985" yWindow="-21390" windowWidth="28995" windowHeight="20055" xr2:uid="{6CF1A792-55F6-4EFF-A83A-261B71252191}"/>
   </bookViews>
   <sheets>
     <sheet name="Court Event" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="490">
   <si>
     <t>Property Type</t>
   </si>
@@ -1793,6 +1793,18 @@
   </si>
   <si>
     <t>/nola:CaseInitiationExchange/CourtCase/j:CaseAugmentation/j:CaseDefendantParty/EntityPerson/nola-ext:PersonAugmentation/nc:PersonEmploymentAssociation/nc:EmploymentStatus/nc:StatusDescriptionText</t>
+  </si>
+  <si>
+    <t>CourtEventCodeText</t>
+  </si>
+  <si>
+    <t>nola-ext:CourtEventTypeText</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/j:CourtEvent/nola-ext:CourtEventAugmentation/nola-ext:CourtEventTypeCode</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/j:CourtEvent/nola-ext:CourtEventAugmentation/nola-ext:CourtEventTypeText</t>
   </si>
 </sst>
 </file>
@@ -1951,7 +1963,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2009,6 +2021,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2872,13 +2893,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18CFC728-CFAD-4708-B4DA-65E1AE154AFA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O93"/>
+  <dimension ref="A1:O94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="I59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="G56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L93" sqref="L93"/>
+      <selection pane="bottomRight" activeCell="L94" sqref="L94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4860,7 +4881,7 @@
       <c r="H54" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="I54" s="9" t="s">
+      <c r="I54" s="21" t="s">
         <v>264</v>
       </c>
       <c r="J54" s="9" t="s">
@@ -4869,8 +4890,8 @@
       <c r="K54" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="L54" s="9" t="s">
-        <v>53</v>
+      <c r="L54" s="21" t="s">
+        <v>488</v>
       </c>
       <c r="M54" s="9"/>
       <c r="N54" s="9"/>
@@ -6382,6 +6403,47 @@
         <v>448</v>
       </c>
     </row>
+    <row r="94" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A94" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C94" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="D94" s="23" t="s">
+        <v>486</v>
+      </c>
+      <c r="E94" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F94" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="G94" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H94" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="I94" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="J94" s="23" t="s">
+        <v>487</v>
+      </c>
+      <c r="K94" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="L94" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="M94" s="23"/>
+      <c r="N94" s="23"/>
+      <c r="O94" s="23"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Made CourtEventSequenceID mandataory. Made CourtEventTypeCode an  int.
</commit_message>
<xml_diff>
--- a/schemas/CourtEvent_iepd/artifacts/CourtEvent_MappingSpreadsheet.xlsx
+++ b/schemas/CourtEvent_iepd/artifacts/CourtEvent_MappingSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\CourtEvent_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2336F03-3B0E-41A9-AEF0-4F2580DA72D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF2C4B3-D3D1-4EB5-8B2A-813F99C11C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14985" yWindow="-21390" windowWidth="28995" windowHeight="20055" xr2:uid="{6CF1A792-55F6-4EFF-A83A-261B71252191}"/>
+    <workbookView xWindow="-4080" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{6CF1A792-55F6-4EFF-A83A-261B71252191}"/>
   </bookViews>
   <sheets>
     <sheet name="Court Event" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="497">
   <si>
     <t>Property Type</t>
   </si>
@@ -1805,6 +1805,27 @@
   </si>
   <si>
     <t>/nola:CourtEventExchange/j:CourtEvent/nola-ext:CourtEventAugmentation/nola-ext:CourtEventTypeText</t>
+  </si>
+  <si>
+    <t>CourtEventSequenceID</t>
+  </si>
+  <si>
+    <t>j:CourtEventSequenceID</t>
+  </si>
+  <si>
+    <t>/nola:CourtEventExchange/j:CourtEvent/j:CourtEventSequenceID</t>
+  </si>
+  <si>
+    <t>A unique identifier for a court event/hearing.</t>
+  </si>
+  <si>
+    <t>A description of a specific type of court event.</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>niem-xs:int</t>
   </si>
 </sst>
 </file>
@@ -1963,7 +1984,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1998,22 +2019,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -2030,6 +2039,20 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2572,8 +2595,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D1C00DE-EF4F-483A-9AEE-9A164B2AF960}" name="MappingSpreadsheet" displayName="MappingSpreadsheet" ref="A1:O78" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
-  <autoFilter ref="A1:O78" xr:uid="{B09137D3-E1F4-4790-A6C1-6986B28644D7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D1C00DE-EF4F-483A-9AEE-9A164B2AF960}" name="MappingSpreadsheet" displayName="MappingSpreadsheet" ref="A1:O95" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O95">
+    <sortCondition ref="C2:C95"/>
+    <sortCondition ref="D2:D95"/>
+  </sortState>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{DDD07387-8786-4201-81D4-D049D1BB39CD}" name="Property Type" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{8412112B-6506-4FC5-A8DB-BBBB368BBCE4}" name="ID" dataDxfId="13"/>
@@ -2893,13 +2919,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18CFC728-CFAD-4708-B4DA-65E1AE154AFA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O94"/>
+  <dimension ref="A1:O95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="G56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L94" sqref="L94"/>
+      <selection pane="bottomRight" activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4881,16 +4907,16 @@
       <c r="H54" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="I54" s="21" t="s">
+      <c r="I54" s="17" t="s">
         <v>264</v>
       </c>
       <c r="J54" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="K54" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="L54" s="21" t="s">
+      <c r="K54" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="L54" s="17" t="s">
         <v>488</v>
       </c>
       <c r="M54" s="9"/>
@@ -4898,1551 +4924,1597 @@
       <c r="O54" s="9"/>
     </row>
     <row r="55" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>486</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>494</v>
+      </c>
+      <c r="G55" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H55" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="I55" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="J55" s="19" t="s">
+        <v>487</v>
+      </c>
+      <c r="K55" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="L55" s="19" t="s">
+        <v>489</v>
+      </c>
+      <c r="M55" s="19"/>
+      <c r="N55" s="19"/>
+      <c r="O55" s="19"/>
+    </row>
+    <row r="56" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B56" s="8" t="s">
         <v>266</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="G55" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K55" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="L55" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="M55" s="9"/>
-      <c r="N55" s="9"/>
-      <c r="O55" s="9"/>
-    </row>
-    <row r="56" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>270</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="D56" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>50</v>
+      <c r="D56" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="G56" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="G56" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H56" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="I56" s="9" t="s">
-        <v>273</v>
-      </c>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
       <c r="J56" s="9" t="s">
-        <v>274</v>
+        <v>32</v>
       </c>
       <c r="K56" s="9" t="s">
-        <v>223</v>
+        <v>33</v>
       </c>
       <c r="L56" s="9" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="M56" s="9"/>
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
     </row>
     <row r="57" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="I57" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="K57" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="L57" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
+      <c r="O57" s="9"/>
+    </row>
+    <row r="58" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>490</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>493</v>
+      </c>
+      <c r="G58" s="15" t="s">
+        <v>495</v>
+      </c>
+      <c r="H58" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="I58" s="15"/>
+      <c r="J58" s="19" t="s">
+        <v>491</v>
+      </c>
+      <c r="K58" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="L58" s="19" t="s">
+        <v>492</v>
+      </c>
+      <c r="M58" s="19"/>
+      <c r="N58" s="19"/>
+      <c r="O58" s="19"/>
+    </row>
+    <row r="59" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D59" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E57" s="5"/>
-      <c r="F57" s="4" t="s">
+      <c r="E59" s="5"/>
+      <c r="F59" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="G57" s="5"/>
-      <c r="H57" s="4" t="s">
+      <c r="G59" s="5"/>
+      <c r="H59" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="4"/>
-      <c r="O57" s="4"/>
-    </row>
-    <row r="58" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="10" t="s">
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+    </row>
+    <row r="60" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B60" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C60" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="D58" s="11" t="s">
+      <c r="D60" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E58" s="11" t="s">
+      <c r="E60" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="F60" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="G58" s="11" t="s">
+      <c r="G60" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9" t="s">
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="K58" s="9" t="s">
+      <c r="K60" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="L58" s="9" t="s">
+      <c r="L60" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="M58" s="9"/>
-      <c r="N58" s="9"/>
-      <c r="O58" s="9"/>
-    </row>
-    <row r="59" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="10" t="s">
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
+      <c r="O60" s="9"/>
+    </row>
+    <row r="61" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B61" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C61" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="D59" s="11" t="s">
+      <c r="D61" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="E61" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="F59" s="9" t="s">
+      <c r="F61" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="G61" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="9"/>
-      <c r="L59" s="9"/>
-      <c r="M59" s="9"/>
-      <c r="N59" s="9"/>
-      <c r="O59" s="9"/>
-    </row>
-    <row r="60" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E60" s="5"/>
-      <c r="F60" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="G60" s="5"/>
-      <c r="H60" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="4" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H61" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="I61" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="J61" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="K61" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="L61" s="9" t="s">
-        <v>295</v>
-      </c>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
+      <c r="L61" s="9"/>
       <c r="M61" s="9"/>
       <c r="N61" s="9"/>
       <c r="O61" s="9"/>
     </row>
     <row r="62" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="C62" s="9" t="s">
+      <c r="A62" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>392</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" s="16"/>
+      <c r="F62" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="G62" s="16"/>
+      <c r="H62" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="15" t="s">
+        <v>405</v>
+      </c>
+      <c r="M62" s="15"/>
+      <c r="N62" s="15"/>
+      <c r="O62" s="22"/>
+    </row>
+    <row r="63" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A63" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>396</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>397</v>
+      </c>
+      <c r="G63" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="H63" s="15" t="s">
+        <v>396</v>
+      </c>
+      <c r="I63" s="15" t="s">
+        <v>398</v>
+      </c>
+      <c r="J63" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="K63" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="L63" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="M63" s="22"/>
+      <c r="N63" s="22"/>
+      <c r="O63" s="22"/>
+    </row>
+    <row r="64" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>400</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>401</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F64" s="15" t="s">
+        <v>402</v>
+      </c>
+      <c r="G64" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="H64" s="15" t="s">
+        <v>401</v>
+      </c>
+      <c r="I64" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="J64" s="15" t="s">
+        <v>404</v>
+      </c>
+      <c r="K64" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="L64" s="15" t="s">
+        <v>407</v>
+      </c>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15"/>
+      <c r="O64" s="22"/>
+    </row>
+    <row r="65" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A65" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>435</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>436</v>
+      </c>
+      <c r="E65" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>437</v>
+      </c>
+      <c r="G65" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H65" s="15" t="s">
+        <v>436</v>
+      </c>
+      <c r="I65" s="15" t="s">
+        <v>438</v>
+      </c>
+      <c r="J65" s="15" t="s">
+        <v>439</v>
+      </c>
+      <c r="K65" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="L65" s="15" t="s">
+        <v>484</v>
+      </c>
+      <c r="M65" s="15" t="s">
+        <v>440</v>
+      </c>
+      <c r="N65" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="O65" s="22"/>
+    </row>
+    <row r="66" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A66" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>435</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>443</v>
+      </c>
+      <c r="E66" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>444</v>
+      </c>
+      <c r="G66" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H66" s="15" t="s">
+        <v>443</v>
+      </c>
+      <c r="I66" s="15" t="s">
+        <v>445</v>
+      </c>
+      <c r="J66" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="K66" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="L66" s="15" t="s">
+        <v>485</v>
+      </c>
+      <c r="M66" s="15" t="s">
+        <v>447</v>
+      </c>
+      <c r="N66" s="15" t="s">
+        <v>448</v>
+      </c>
+      <c r="O66" s="22"/>
+    </row>
+    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A67" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="D62" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="E62" s="9" t="s">
+      <c r="D67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67" s="5"/>
+      <c r="F67" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="G67" s="5"/>
+      <c r="H67" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A68" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E68" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F62" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="G62" s="9" t="s">
+      <c r="F68" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="G68" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H62" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="I62" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="J62" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="K62" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="L62" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="M62" s="9"/>
-      <c r="N62" s="9"/>
-      <c r="O62" s="9"/>
-    </row>
-    <row r="63" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E63" s="5"/>
-      <c r="F63" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="G63" s="5"/>
-      <c r="H63" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="L63" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="G64" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H64" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I64" s="9"/>
-      <c r="J64" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="K64" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="L64" s="9"/>
-      <c r="M64" s="9"/>
-      <c r="N64" s="9"/>
-      <c r="O64" s="9"/>
-    </row>
-    <row r="65" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E65" s="5"/>
-      <c r="F65" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="G65" s="5"/>
-      <c r="H65" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
-      <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
-    </row>
-    <row r="66" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E66" s="5"/>
-      <c r="F66" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="G66" s="5"/>
-      <c r="H66" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-    </row>
-    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="H67" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="I67" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="J67" s="9" t="s">
-        <v>320</v>
-      </c>
-      <c r="K67" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="L67" s="9" t="s">
-        <v>322</v>
-      </c>
-      <c r="M67" s="9"/>
-      <c r="N67" s="9"/>
-      <c r="O67" s="9"/>
-    </row>
-    <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="E68" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="G68" s="11" t="s">
-        <v>326</v>
-      </c>
       <c r="H68" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I68" s="9"/>
+        <v>292</v>
+      </c>
+      <c r="I68" s="9" t="s">
+        <v>294</v>
+      </c>
       <c r="J68" s="9" t="s">
-        <v>327</v>
+        <v>81</v>
       </c>
       <c r="K68" s="9" t="s">
-        <v>328</v>
+        <v>82</v>
       </c>
       <c r="L68" s="9" t="s">
-        <v>329</v>
+        <v>295</v>
       </c>
       <c r="M68" s="9"/>
       <c r="N68" s="9"/>
       <c r="O68" s="9"/>
     </row>
     <row r="69" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="I69" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J69" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="K69" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="L69" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9"/>
+      <c r="O69" s="9"/>
+    </row>
+    <row r="70" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A70" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B69" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="D69" s="4" t="s">
+      <c r="B70" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E69" s="5"/>
-      <c r="F69" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="G69" s="5"/>
-      <c r="H69" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="I69" s="4"/>
-      <c r="J69" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="K69" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="L69" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="M69" s="4"/>
-      <c r="N69" s="4"/>
-      <c r="O69" s="4"/>
-    </row>
-    <row r="70" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F70" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="G70" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="H70" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="I70" s="9" t="s">
-        <v>336</v>
-      </c>
-      <c r="J70" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="K70" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="L70" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="M70" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="N70" s="9"/>
-      <c r="O70" s="9"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="G70" s="5"/>
+      <c r="H70" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="L70" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="71" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="7" t="s">
-        <v>3</v>
+      <c r="A71" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>340</v>
+        <v>305</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>324</v>
+        <v>167</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="E71" s="9" t="s">
-        <v>44</v>
+        <v>306</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>288</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>342</v>
-      </c>
-      <c r="G71" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="G71" s="11" t="s">
         <v>26</v>
       </c>
       <c r="H71" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="I71" s="9" t="s">
-        <v>343</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="I71" s="9"/>
       <c r="J71" s="9" t="s">
-        <v>344</v>
+        <v>307</v>
       </c>
       <c r="K71" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="L71" s="9" t="s">
-        <v>346</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="L71" s="9"/>
       <c r="M71" s="9"/>
       <c r="N71" s="9"/>
-      <c r="O71" s="9" t="s">
+      <c r="O71" s="9"/>
+    </row>
+    <row r="72" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A72" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E72" s="5"/>
+      <c r="F72" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="G72" s="5"/>
+      <c r="H72" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4"/>
+    </row>
+    <row r="73" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A73" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F72" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="G72" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H72" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="I72" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="J72" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="K72" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="L72" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="M72" s="9"/>
-      <c r="N72" s="9"/>
-      <c r="O72" s="9"/>
-    </row>
-    <row r="73" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>354</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="G73" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H73" s="9" t="s">
-        <v>354</v>
-      </c>
-      <c r="I73" s="9" t="s">
-        <v>356</v>
-      </c>
-      <c r="J73" s="9" t="s">
-        <v>357</v>
-      </c>
-      <c r="K73" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="L73" s="9" t="s">
-        <v>358</v>
-      </c>
-      <c r="M73" s="9"/>
-      <c r="N73" s="9"/>
-      <c r="O73" s="9" t="s">
+      <c r="D73" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E73" s="5"/>
+      <c r="F73" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="G73" s="5"/>
+      <c r="H73" s="4" t="s">
         <v>313</v>
       </c>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4"/>
     </row>
     <row r="74" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>359</v>
+        <v>315</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>360</v>
+        <v>316</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>44</v>
+        <v>317</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>361</v>
+        <v>318</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>360</v>
+        <v>316</v>
       </c>
       <c r="I74" s="9" t="s">
-        <v>362</v>
+        <v>319</v>
       </c>
       <c r="J74" s="9" t="s">
-        <v>363</v>
+        <v>320</v>
       </c>
       <c r="K74" s="9" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="L74" s="9" t="s">
-        <v>364</v>
+        <v>322</v>
       </c>
       <c r="M74" s="9"/>
       <c r="N74" s="9"/>
-      <c r="O74" s="9" t="s">
+      <c r="O74" s="9"/>
+    </row>
+    <row r="75" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A75" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="C75" s="9" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="C75" s="9" t="s">
+      <c r="D75" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="D75" s="9" t="s">
-        <v>366</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>44</v>
+      <c r="E75" s="11" t="s">
+        <v>324</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="G75" s="9" t="s">
-        <v>26</v>
+        <v>325</v>
+      </c>
+      <c r="G75" s="11" t="s">
+        <v>326</v>
       </c>
       <c r="H75" s="9" t="s">
-        <v>366</v>
-      </c>
-      <c r="I75" s="9" t="s">
-        <v>368</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="I75" s="9"/>
       <c r="J75" s="9" t="s">
-        <v>369</v>
+        <v>327</v>
       </c>
       <c r="K75" s="9" t="s">
-        <v>94</v>
+        <v>328</v>
       </c>
       <c r="L75" s="9" t="s">
-        <v>370</v>
+        <v>329</v>
       </c>
       <c r="M75" s="9"/>
       <c r="N75" s="9"/>
-      <c r="O75" s="9" t="s">
+      <c r="O75" s="9"/>
+    </row>
+    <row r="76" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A76" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E76" s="16"/>
+      <c r="F76" s="15" t="s">
+        <v>451</v>
+      </c>
+      <c r="G76" s="16"/>
+      <c r="H76" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="15"/>
+      <c r="O76" s="22"/>
+    </row>
+    <row r="77" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A77" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>452</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F77" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="G77" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H77" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="I77" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="J77" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="K77" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="L77" s="15" t="s">
+        <v>478</v>
+      </c>
+      <c r="M77" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="N77" s="15" t="s">
+        <v>458</v>
+      </c>
+      <c r="O77" s="22"/>
+    </row>
+    <row r="78" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A78" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="D78" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="E78" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F78" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="G78" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H78" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="I78" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="J78" s="13" t="s">
+        <v>463</v>
+      </c>
+      <c r="K78" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="L78" s="13" t="s">
+        <v>477</v>
+      </c>
+      <c r="M78" s="13" t="s">
+        <v>464</v>
+      </c>
+      <c r="N78" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="O78" s="24"/>
+    </row>
+    <row r="79" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A79" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="C79" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="E79" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="F79" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="G79" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H79" s="23" t="s">
+        <v>467</v>
+      </c>
+      <c r="I79" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="J79" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="K79" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="L79" s="13" t="s">
+        <v>476</v>
+      </c>
+      <c r="M79" s="13" t="s">
+        <v>472</v>
+      </c>
+      <c r="N79" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="O79" s="14"/>
+    </row>
+    <row r="80" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A80" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>474</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E80" s="16"/>
+      <c r="F80" s="15" t="s">
+        <v>475</v>
+      </c>
+      <c r="G80" s="16"/>
+      <c r="H80" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="15"/>
+      <c r="M80" s="15"/>
+      <c r="N80" s="15"/>
+      <c r="O80" s="14"/>
+    </row>
+    <row r="81" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A81" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>408</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>410</v>
+      </c>
+      <c r="E81" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F81" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="G81" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H81" s="15" t="s">
+        <v>410</v>
+      </c>
+      <c r="I81" s="15" t="s">
+        <v>412</v>
+      </c>
+      <c r="J81" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="K81" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="L81" s="15" t="s">
+        <v>479</v>
+      </c>
+      <c r="M81" s="23" t="s">
+        <v>415</v>
+      </c>
+      <c r="N81" s="23" t="s">
+        <v>416</v>
+      </c>
+      <c r="O81" s="14"/>
+    </row>
+    <row r="82" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A82" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>417</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>418</v>
+      </c>
+      <c r="E82" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F82" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="G82" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H82" s="15" t="s">
+        <v>418</v>
+      </c>
+      <c r="I82" s="15"/>
+      <c r="J82" s="15" t="s">
+        <v>420</v>
+      </c>
+      <c r="K82" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="L82" s="15" t="s">
+        <v>480</v>
+      </c>
+      <c r="M82" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="N82" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="O82" s="14"/>
+    </row>
+    <row r="83" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A83" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="D83" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="E83" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F83" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="G83" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H83" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="I83" s="15" t="s">
+        <v>426</v>
+      </c>
+      <c r="J83" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="K83" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="L83" s="15" t="s">
+        <v>483</v>
+      </c>
+      <c r="M83" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="N83" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="O83" s="14"/>
+    </row>
+    <row r="84" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A84" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>429</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="E84" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F84" s="15" t="s">
+        <v>431</v>
+      </c>
+      <c r="G84" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H84" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="I84" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="J84" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="K84" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="L84" s="15" t="s">
+        <v>481</v>
+      </c>
+      <c r="M84" s="15" t="s">
+        <v>433</v>
+      </c>
+      <c r="N84" s="15" t="s">
+        <v>434</v>
+      </c>
+      <c r="O84" s="14"/>
+    </row>
+    <row r="85" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A85" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E85" s="5"/>
+      <c r="F85" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="G85" s="5"/>
+      <c r="H85" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="K85" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="L85" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="M85" s="4"/>
+      <c r="N85" s="4"/>
+      <c r="O85" s="25"/>
+    </row>
+    <row r="86" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A86" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="D86" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H86" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="I86" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="J86" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="K86" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="L86" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="M86" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="N86" s="9"/>
+      <c r="O86" s="20"/>
+    </row>
+    <row r="87" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A87" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="G87" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H87" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="I87" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="J87" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="K87" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="L87" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="M87" s="9"/>
+      <c r="N87" s="9"/>
+      <c r="O87" s="20" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B76" s="8" t="s">
+    <row r="88" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A88" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="G88" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H88" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="I88" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="J88" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="K88" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="L88" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="M88" s="9"/>
+      <c r="N88" s="9"/>
+      <c r="O88" s="20"/>
+    </row>
+    <row r="89" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A89" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H89" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="I89" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="J89" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="K89" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="L89" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="M89" s="9"/>
+      <c r="N89" s="9"/>
+      <c r="O89" s="20" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A90" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H90" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="I90" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="J90" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="K90" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="L90" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="M90" s="9"/>
+      <c r="N90" s="9"/>
+      <c r="O90" s="20" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A91" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H91" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="I91" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="J91" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="K91" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="L91" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="M91" s="9"/>
+      <c r="N91" s="9"/>
+      <c r="O91" s="20" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A92" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C92" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="D76" s="9" t="s">
+      <c r="D92" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="E76" s="9" t="s">
+      <c r="E92" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F76" s="9" t="s">
+      <c r="F92" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="G76" s="9" t="s">
+      <c r="G92" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="H76" s="9" t="s">
+      <c r="H92" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="I76" s="9" t="s">
+      <c r="I92" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="J76" s="9" t="s">
+      <c r="J92" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="K76" s="9" t="s">
+      <c r="K92" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="L76" s="9" t="s">
+      <c r="L92" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="M76" s="9"/>
-      <c r="N76" s="9"/>
-      <c r="O76" s="9"/>
-    </row>
-    <row r="77" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B77" s="8" t="s">
+      <c r="M92" s="9"/>
+      <c r="N92" s="9"/>
+      <c r="O92" s="20"/>
+    </row>
+    <row r="93" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A93" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C93" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="D77" s="9" t="s">
+      <c r="D93" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="E93" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F77" s="9" t="s">
+      <c r="F93" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="G77" s="9" t="s">
+      <c r="G93" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H77" s="9" t="s">
+      <c r="H93" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="I77" s="9" t="s">
+      <c r="I93" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="J77" s="9"/>
-      <c r="K77" s="9"/>
-      <c r="L77" s="9" t="s">
+      <c r="J93" s="9"/>
+      <c r="K93" s="9"/>
+      <c r="L93" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="M77" s="9"/>
-      <c r="N77" s="9"/>
-      <c r="O77" s="9"/>
-    </row>
-    <row r="78" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A78" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B78" s="13" t="s">
+      <c r="M93" s="9"/>
+      <c r="N93" s="9"/>
+      <c r="O93" s="20"/>
+    </row>
+    <row r="94" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A94" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C94" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="D78" s="14" t="s">
+      <c r="D94" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="E78" s="14" t="s">
+      <c r="E94" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F78" s="14" t="s">
+      <c r="F94" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="G78" s="14" t="s">
+      <c r="G94" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="H78" s="14" t="s">
+      <c r="H94" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="I78" s="14" t="s">
+      <c r="I94" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="J78" s="14" t="s">
+      <c r="J94" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="K78" s="14" t="s">
+      <c r="K94" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="L78" s="14" t="s">
+      <c r="L94" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="M78" s="14"/>
-      <c r="N78" s="14"/>
-      <c r="O78" s="14"/>
-    </row>
-    <row r="79" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A79" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B79" s="16"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="17" t="s">
+      <c r="M94" s="9"/>
+      <c r="N94" s="9"/>
+      <c r="O94" s="9"/>
+    </row>
+    <row r="95" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A95" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95" s="15"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="16" t="s">
         <v>388</v>
       </c>
-      <c r="E79" s="17" t="s">
+      <c r="E95" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F79" s="17" t="s">
+      <c r="F95" s="16" t="s">
         <v>389</v>
       </c>
-      <c r="G79" s="17" t="s">
+      <c r="G95" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="H79" s="18" t="s">
+      <c r="H95" s="22" t="s">
         <v>388</v>
       </c>
-      <c r="I79" s="16"/>
-      <c r="J79" s="16" t="s">
+      <c r="I95" s="15"/>
+      <c r="J95" s="15" t="s">
         <v>390</v>
       </c>
-      <c r="K79" s="16" t="s">
+      <c r="K95" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="L79" s="16" t="s">
+      <c r="L95" s="15" t="s">
         <v>482</v>
       </c>
-      <c r="M79" s="16"/>
-      <c r="N79" s="16"/>
-      <c r="O79" s="18"/>
-    </row>
-    <row r="80" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A80" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" s="19" t="s">
-        <v>392</v>
-      </c>
-      <c r="C80" s="19" t="s">
-        <v>393</v>
-      </c>
-      <c r="D80" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E80" s="20"/>
-      <c r="F80" s="19" t="s">
-        <v>394</v>
-      </c>
-      <c r="G80" s="20"/>
-      <c r="H80" s="19" t="s">
-        <v>393</v>
-      </c>
-      <c r="I80" s="19"/>
-      <c r="J80" s="19"/>
-      <c r="K80" s="19"/>
-      <c r="L80" s="19" t="s">
-        <v>405</v>
-      </c>
-      <c r="M80" s="19"/>
-      <c r="N80" s="19"/>
-      <c r="O80" s="18"/>
-    </row>
-    <row r="81" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A81" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81" s="19" t="s">
-        <v>395</v>
-      </c>
-      <c r="C81" s="19" t="s">
-        <v>393</v>
-      </c>
-      <c r="D81" s="19" t="s">
-        <v>396</v>
-      </c>
-      <c r="E81" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F81" s="19" t="s">
-        <v>397</v>
-      </c>
-      <c r="G81" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="H81" s="19" t="s">
-        <v>396</v>
-      </c>
-      <c r="I81" s="19" t="s">
-        <v>398</v>
-      </c>
-      <c r="J81" s="19" t="s">
-        <v>399</v>
-      </c>
-      <c r="K81" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="L81" s="19" t="s">
-        <v>406</v>
-      </c>
-      <c r="M81" s="18"/>
-      <c r="N81" s="18"/>
-      <c r="O81" s="18"/>
-    </row>
-    <row r="82" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82" s="19" t="s">
-        <v>400</v>
-      </c>
-      <c r="C82" s="19" t="s">
-        <v>393</v>
-      </c>
-      <c r="D82" s="19" t="s">
-        <v>401</v>
-      </c>
-      <c r="E82" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F82" s="19" t="s">
-        <v>402</v>
-      </c>
-      <c r="G82" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="H82" s="19" t="s">
-        <v>401</v>
-      </c>
-      <c r="I82" s="19" t="s">
-        <v>403</v>
-      </c>
-      <c r="J82" s="19" t="s">
-        <v>404</v>
-      </c>
-      <c r="K82" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="L82" s="19" t="s">
-        <v>407</v>
-      </c>
-      <c r="M82" s="19"/>
-      <c r="N82" s="19"/>
-      <c r="O82" s="18"/>
-    </row>
-    <row r="83" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A83" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B83" s="19" t="s">
-        <v>449</v>
-      </c>
-      <c r="C83" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="D83" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E83" s="20"/>
-      <c r="F83" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="G83" s="20"/>
-      <c r="H83" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="I83" s="19"/>
-      <c r="J83" s="19"/>
-      <c r="K83" s="19"/>
-      <c r="L83" s="19"/>
-      <c r="M83" s="19"/>
-      <c r="N83" s="19"/>
-    </row>
-    <row r="84" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A84" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B84" s="19" t="s">
-        <v>452</v>
-      </c>
-      <c r="C84" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="D84" s="19" t="s">
-        <v>453</v>
-      </c>
-      <c r="E84" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F84" s="19" t="s">
-        <v>454</v>
-      </c>
-      <c r="G84" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H84" s="19" t="s">
-        <v>453</v>
-      </c>
-      <c r="I84" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="J84" s="19" t="s">
-        <v>456</v>
-      </c>
-      <c r="K84" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="L84" s="19" t="s">
-        <v>478</v>
-      </c>
-      <c r="M84" s="19" t="s">
-        <v>457</v>
-      </c>
-      <c r="N84" s="19" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A85" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B85" s="19" t="s">
-        <v>459</v>
-      </c>
-      <c r="C85" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="D85" s="19" t="s">
-        <v>460</v>
-      </c>
-      <c r="E85" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F85" s="19" t="s">
-        <v>461</v>
-      </c>
-      <c r="G85" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H85" s="19" t="s">
-        <v>460</v>
-      </c>
-      <c r="I85" s="19" t="s">
-        <v>462</v>
-      </c>
-      <c r="J85" s="19" t="s">
-        <v>463</v>
-      </c>
-      <c r="K85" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="L85" s="19" t="s">
-        <v>477</v>
-      </c>
-      <c r="M85" s="19" t="s">
-        <v>464</v>
-      </c>
-      <c r="N85" s="19" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A86" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B86" s="19" t="s">
-        <v>466</v>
-      </c>
-      <c r="C86" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="D86" s="19" t="s">
-        <v>467</v>
-      </c>
-      <c r="E86" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="F86" s="19" t="s">
-        <v>468</v>
-      </c>
-      <c r="G86" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H86" s="19" t="s">
-        <v>467</v>
-      </c>
-      <c r="I86" s="19" t="s">
-        <v>469</v>
-      </c>
-      <c r="J86" s="19" t="s">
-        <v>470</v>
-      </c>
-      <c r="K86" s="19" t="s">
-        <v>471</v>
-      </c>
-      <c r="L86" s="19" t="s">
-        <v>476</v>
-      </c>
-      <c r="M86" s="19" t="s">
-        <v>472</v>
-      </c>
-      <c r="N86" s="19" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A87" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B87" s="19" t="s">
-        <v>474</v>
-      </c>
-      <c r="C87" s="19" t="s">
-        <v>409</v>
-      </c>
-      <c r="D87" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E87" s="20"/>
-      <c r="F87" s="19" t="s">
-        <v>475</v>
-      </c>
-      <c r="G87" s="20"/>
-      <c r="H87" s="19" t="s">
-        <v>409</v>
-      </c>
-      <c r="I87" s="19"/>
-      <c r="J87" s="19"/>
-      <c r="K87" s="19"/>
-      <c r="L87" s="19"/>
-      <c r="M87" s="19"/>
-      <c r="N87" s="19"/>
-    </row>
-    <row r="88" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A88" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B88" s="19" t="s">
-        <v>408</v>
-      </c>
-      <c r="C88" s="19" t="s">
-        <v>409</v>
-      </c>
-      <c r="D88" s="19" t="s">
-        <v>410</v>
-      </c>
-      <c r="E88" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="F88" s="19" t="s">
-        <v>411</v>
-      </c>
-      <c r="G88" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H88" s="19" t="s">
-        <v>410</v>
-      </c>
-      <c r="I88" s="19" t="s">
-        <v>412</v>
-      </c>
-      <c r="J88" s="19" t="s">
-        <v>413</v>
-      </c>
-      <c r="K88" s="19" t="s">
-        <v>414</v>
-      </c>
-      <c r="L88" s="19" t="s">
-        <v>479</v>
-      </c>
-      <c r="M88" s="19" t="s">
-        <v>415</v>
-      </c>
-      <c r="N88" s="19" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A89" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B89" s="19" t="s">
-        <v>417</v>
-      </c>
-      <c r="C89" s="19" t="s">
-        <v>409</v>
-      </c>
-      <c r="D89" s="19" t="s">
-        <v>418</v>
-      </c>
-      <c r="E89" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F89" s="19" t="s">
-        <v>419</v>
-      </c>
-      <c r="G89" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H89" s="19" t="s">
-        <v>418</v>
-      </c>
-      <c r="I89" s="19"/>
-      <c r="J89" s="19" t="s">
-        <v>420</v>
-      </c>
-      <c r="K89" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="L89" s="19" t="s">
-        <v>480</v>
-      </c>
-      <c r="M89" s="19" t="s">
-        <v>421</v>
-      </c>
-      <c r="N89" s="19" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A90" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B90" s="19" t="s">
-        <v>423</v>
-      </c>
-      <c r="C90" s="19" t="s">
-        <v>409</v>
-      </c>
-      <c r="D90" s="19" t="s">
-        <v>424</v>
-      </c>
-      <c r="E90" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F90" s="19" t="s">
-        <v>425</v>
-      </c>
-      <c r="G90" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H90" s="19" t="s">
-        <v>424</v>
-      </c>
-      <c r="I90" s="19" t="s">
-        <v>426</v>
-      </c>
-      <c r="J90" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="K90" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="L90" s="19" t="s">
-        <v>483</v>
-      </c>
-      <c r="M90" s="19" t="s">
-        <v>427</v>
-      </c>
-      <c r="N90" s="19" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A91" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B91" s="19" t="s">
-        <v>429</v>
-      </c>
-      <c r="C91" s="19" t="s">
-        <v>409</v>
-      </c>
-      <c r="D91" s="19" t="s">
-        <v>430</v>
-      </c>
-      <c r="E91" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F91" s="19" t="s">
-        <v>431</v>
-      </c>
-      <c r="G91" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H91" s="19" t="s">
-        <v>430</v>
-      </c>
-      <c r="I91" s="19" t="s">
-        <v>432</v>
-      </c>
-      <c r="J91" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="K91" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="L91" s="19" t="s">
-        <v>481</v>
-      </c>
-      <c r="M91" s="19" t="s">
-        <v>433</v>
-      </c>
-      <c r="N91" s="19" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A92" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B92" s="19" t="s">
-        <v>305</v>
-      </c>
-      <c r="C92" s="19" t="s">
-        <v>435</v>
-      </c>
-      <c r="D92" s="19" t="s">
-        <v>436</v>
-      </c>
-      <c r="E92" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F92" s="19" t="s">
-        <v>437</v>
-      </c>
-      <c r="G92" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H92" s="19" t="s">
-        <v>436</v>
-      </c>
-      <c r="I92" s="19" t="s">
-        <v>438</v>
-      </c>
-      <c r="J92" s="19" t="s">
-        <v>439</v>
-      </c>
-      <c r="K92" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="L92" s="19" t="s">
-        <v>484</v>
-      </c>
-      <c r="M92" s="19" t="s">
-        <v>440</v>
-      </c>
-      <c r="N92" s="19" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A93" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B93" s="19" t="s">
-        <v>442</v>
-      </c>
-      <c r="C93" s="19" t="s">
-        <v>435</v>
-      </c>
-      <c r="D93" s="19" t="s">
-        <v>443</v>
-      </c>
-      <c r="E93" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F93" s="19" t="s">
-        <v>444</v>
-      </c>
-      <c r="G93" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H93" s="19" t="s">
-        <v>443</v>
-      </c>
-      <c r="I93" s="19" t="s">
-        <v>445</v>
-      </c>
-      <c r="J93" s="19" t="s">
-        <v>446</v>
-      </c>
-      <c r="K93" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="L93" s="19" t="s">
-        <v>485</v>
-      </c>
-      <c r="M93" s="19" t="s">
-        <v>447</v>
-      </c>
-      <c r="N93" s="19" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A94" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B94" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C94" s="23" t="s">
-        <v>257</v>
-      </c>
-      <c r="D94" s="23" t="s">
-        <v>486</v>
-      </c>
-      <c r="E94" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F94" s="23" t="s">
-        <v>263</v>
-      </c>
-      <c r="G94" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H94" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="I94" s="19" t="s">
-        <v>264</v>
-      </c>
-      <c r="J94" s="23" t="s">
-        <v>487</v>
-      </c>
-      <c r="K94" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="L94" s="23" t="s">
-        <v>489</v>
-      </c>
-      <c r="M94" s="23"/>
-      <c r="N94" s="23"/>
-      <c r="O94" s="23"/>
+      <c r="M95" s="15"/>
+      <c r="N95" s="15"/>
+      <c r="O95" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>